<commit_message>
Update PG Machine Excel files
Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/PG - machine v2.xlsx
+++ b/PG - machine v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fbianchi/Documents/PG Machine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0153A8A7-3616-F149-A74F-F10EC683CD4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4EFA55-8985-F04C-9241-B863C709AEB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4420" yWindow="660" windowWidth="24980" windowHeight="17160" xr2:uid="{3AC6B55B-9A84-B24A-BBC1-264510FBEEC5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
   <si>
     <t>Codelco</t>
   </si>
@@ -86,13 +86,16 @@
     <t>Valor</t>
   </si>
   <si>
-    <t>Categoria</t>
-  </si>
-  <si>
     <t>Asset Mgmgt</t>
   </si>
   <si>
     <t>ITSM</t>
+  </si>
+  <si>
+    <t>InADvance</t>
+  </si>
+  <si>
+    <t>Partner</t>
   </si>
 </sst>
 </file>
@@ -486,7 +489,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="178" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D13"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -504,7 +507,7 @@
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -512,7 +515,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -526,7 +529,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -540,7 +543,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>0</v>
@@ -554,13 +557,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1">
         <v>200000</v>
@@ -568,7 +571,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
@@ -582,7 +585,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
@@ -596,7 +599,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
@@ -610,7 +613,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
@@ -624,7 +627,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>10</v>
@@ -638,7 +641,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>10</v>
@@ -652,7 +655,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>11</v>
@@ -666,7 +669,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>11</v>

</xml_diff>